<commit_message>
changed column width to make display clear
</commit_message>
<xml_diff>
--- a/src/api/api3/test-case-planner.xlsx
+++ b/src/api/api3/test-case-planner.xlsx
@@ -887,9 +887,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="14" width="39.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="48.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="54.29071428571429" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="14" width="58.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="37.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="69.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="39.75" customFormat="1" s="1">

</xml_diff>